<commit_message>
debug_backplane: fixup BOM for two new switches
</commit_message>
<xml_diff>
--- a/hardware/debug_backplane/rev_c/debug_backplane_bom.xlsx
+++ b/hardware/debug_backplane/rev_c/debug_backplane_bom.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-48200" yWindow="620" windowWidth="43800" windowHeight="26980" tabRatio="500"/>
+    <workbookView xWindow="5440" yWindow="560" windowWidth="40520" windowHeight="27460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -270,9 +270,6 @@
     <t>0603-RES</t>
   </si>
   <si>
-    <t>R27, R28, R29, R30</t>
-  </si>
-  <si>
     <t>RES SMD 1.5K OHM 5% 1/10W 0603</t>
   </si>
   <si>
@@ -294,9 +291,6 @@
     <t>ARRAY-CONVEX-0603-4</t>
   </si>
   <si>
-    <t>R31, R32, R33, R34</t>
-  </si>
-  <si>
     <t>RES ARRAY 4 RES 1.8K OHM 1206</t>
   </si>
   <si>
@@ -312,9 +306,6 @@
     <t>100kΩ</t>
   </si>
   <si>
-    <t>R64, R65, R66, R67</t>
-  </si>
-  <si>
     <t>RES SMD 100K OHM 1% 1/16W 0402</t>
   </si>
   <si>
@@ -345,9 +336,6 @@
     <t>10kΩ</t>
   </si>
   <si>
-    <t>R35, R36, R37, R38, R39, R40, R41, R42, R43, R44, R45, R46, R47, R48, R49, R50, R51, R52</t>
-  </si>
-  <si>
     <t>RES SMD 10K OHM 5% 1/10W 0603</t>
   </si>
   <si>
@@ -381,9 +369,6 @@
     <t>15kΩ</t>
   </si>
   <si>
-    <t>R61, R62, R63</t>
-  </si>
-  <si>
     <t>RES ARRAY 4 RES 15K OHM 1206</t>
   </si>
   <si>
@@ -393,9 +378,6 @@
     <t>EXB-38V153JV</t>
   </si>
   <si>
-    <t>R53, R54, R55, R56, R57, R58, R59, R60</t>
-  </si>
-  <si>
     <t>RES SMD 15K OHM 1% 1/10W 0603</t>
   </si>
   <si>
@@ -900,9 +882,6 @@
     <t>MMS42</t>
   </si>
   <si>
-    <t>S21, S22</t>
-  </si>
-  <si>
     <t>4PDT - SWITCH SLIDE 4PDT 300MA 30V</t>
   </si>
   <si>
@@ -945,9 +924,6 @@
     <t>SC70-6</t>
   </si>
   <si>
-    <t>S9, S10</t>
-  </si>
-  <si>
     <t>MUX</t>
   </si>
   <si>
@@ -1002,9 +978,6 @@
     <t>PTS645</t>
   </si>
   <si>
-    <t>S3, S4, S5, S6, S7, S8, S20</t>
-  </si>
-  <si>
     <t>Tactile Switch SPST-NO Top Actuated Surface Mount</t>
   </si>
   <si>
@@ -1017,9 +990,6 @@
     <t>RM-SWITCH</t>
   </si>
   <si>
-    <t>S11</t>
-  </si>
-  <si>
     <t>Rotary Switch 6 Position SP6T 500mA (DC) 24VDC Through Hole</t>
   </si>
   <si>
@@ -1047,9 +1017,6 @@
     <t>TDFN4</t>
   </si>
   <si>
-    <t>S12, S13</t>
-  </si>
-  <si>
     <t>High power (2.4 A) high-side switch</t>
   </si>
   <si>
@@ -1062,9 +1029,6 @@
     <t>S-PVQFN-N14-3.5MM</t>
   </si>
   <si>
-    <t>S14, S15, S16, S17, S18</t>
-  </si>
-  <si>
     <t>296-15258-1-ND</t>
   </si>
   <si>
@@ -1149,9 +1113,6 @@
     <t>TE_SSA12/SPDT</t>
   </si>
   <si>
-    <t>S19, S23</t>
-  </si>
-  <si>
     <t>SWITCH SLIDE SPDT 2POS SSA SER</t>
   </si>
   <si>
@@ -1431,13 +1392,52 @@
     <t>732-5316-ND</t>
   </si>
   <si>
-    <t>R68, R69, R70, R71, R72, R73, R74, R75, R76, R77</t>
-  </si>
-  <si>
-    <t>R78, R79, R80, R81, R82, R83</t>
-  </si>
-  <si>
-    <t>R84</t>
+    <t>R27, R28, R29, R30, R31</t>
+  </si>
+  <si>
+    <t>R32, R33, R34, R35</t>
+  </si>
+  <si>
+    <t>R36, R37, R38, R39, R40, R41, R42, R43, R44, R45, R46, R47, R48, R49, R50, R51, R52, R53</t>
+  </si>
+  <si>
+    <t>R54, R55, R56, R57, R58, R59, R60, R61</t>
+  </si>
+  <si>
+    <t>R62, R63, R64</t>
+  </si>
+  <si>
+    <t>R65, R66, R67, R68</t>
+  </si>
+  <si>
+    <t>R69, R70, R71, R72, R73, R74, R75, R76, R77, R78</t>
+  </si>
+  <si>
+    <t>R79, R80, R81, R82, R83, R84</t>
+  </si>
+  <si>
+    <t>R85</t>
+  </si>
+  <si>
+    <t>S7, S8, S9, S10, S11, S12, S13</t>
+  </si>
+  <si>
+    <t>S5, S6</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>S15, S16, S17, S18</t>
+  </si>
+  <si>
+    <t>S19, S20, S21, S22, S23</t>
+  </si>
+  <si>
+    <t>S24, S25</t>
+  </si>
+  <si>
+    <t>S3, S4</t>
   </si>
 </sst>
 </file>
@@ -1567,7 +1567,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1599,6 +1599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1897,8 +1898,8 @@
   <dimension ref="A1:O79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1929,10 +1930,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1962,7 +1963,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -1970,14 +1971,14 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>38</v>
@@ -1986,10 +1987,10 @@
         <v>39</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -1998,10 +1999,10 @@
         <v>43</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -2009,26 +2010,26 @@
         <v>6</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -2037,7 +2038,7 @@
         <v>43</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="O3" s="8"/>
     </row>
@@ -2046,14 +2047,14 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>38</v>
@@ -2062,19 +2063,19 @@
         <v>39</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="O4" s="8"/>
     </row>
@@ -2090,7 +2091,7 @@
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>38</v>
@@ -2127,7 +2128,7 @@
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>38</v>
@@ -2164,7 +2165,7 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>38</v>
@@ -2201,7 +2202,7 @@
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>38</v>
@@ -2231,14 +2232,14 @@
         <v>2</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>38</v>
@@ -2247,10 +2248,10 @@
         <v>39</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -2259,7 +2260,7 @@
         <v>43</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="O9" s="8"/>
     </row>
@@ -2268,14 +2269,14 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>38</v>
@@ -2284,19 +2285,19 @@
         <v>39</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="O10" s="8"/>
     </row>
@@ -2305,14 +2306,14 @@
         <v>1</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>38</v>
@@ -2321,19 +2322,19 @@
         <v>39</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="O11" s="8"/>
     </row>
@@ -2342,35 +2343,35 @@
         <v>2</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F12" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>103</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="O12" s="8"/>
     </row>
@@ -2379,35 +2380,35 @@
         <v>3</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="O13" s="8"/>
     </row>
@@ -2416,35 +2417,35 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="O14" s="8"/>
     </row>
@@ -2453,35 +2454,35 @@
         <v>6</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="O15" s="8"/>
     </row>
@@ -2490,35 +2491,35 @@
         <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="O16" s="8"/>
     </row>
@@ -2527,35 +2528,35 @@
         <v>2</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="O17" s="8"/>
     </row>
@@ -2571,7 +2572,7 @@
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>61</v>
@@ -2601,37 +2602,37 @@
         <v>8</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="O19" s="8"/>
     </row>
@@ -2640,44 +2641,44 @@
         <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="N20" s="11" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="O20" s="8" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -2685,40 +2686,40 @@
         <v>2</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="10" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
@@ -2726,35 +2727,35 @@
         <v>2</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="O22" s="8"/>
     </row>
@@ -2768,7 +2769,7 @@
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>12</v>
@@ -2780,16 +2781,16 @@
         <v>14</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="O23" s="8"/>
     </row>
@@ -2798,35 +2799,35 @@
         <v>1</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="N24" s="6" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="O24" s="8"/>
     </row>
@@ -2835,37 +2836,37 @@
         <v>1</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="O25" s="8"/>
     </row>
@@ -2879,28 +2880,28 @@
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
       <c r="E26" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
       <c r="O26" s="8"/>
     </row>
@@ -2914,28 +2915,28 @@
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
       <c r="E27" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>20</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>433</v>
+        <v>420</v>
       </c>
       <c r="O27" s="8"/>
     </row>
@@ -2949,28 +2950,28 @@
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
       <c r="E28" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="O28" s="8"/>
     </row>
@@ -2979,37 +2980,37 @@
         <v>6</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="N29" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="O29" s="8"/>
     </row>
@@ -3023,28 +3024,28 @@
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
       <c r="E30" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="O30" s="8"/>
     </row>
@@ -3058,25 +3059,25 @@
       <c r="C31" s="6"/>
       <c r="D31" s="7"/>
       <c r="E31" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>18</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="N31" s="12">
         <v>61300311121</v>
@@ -3093,28 +3094,28 @@
       <c r="C32" s="6"/>
       <c r="D32" s="7"/>
       <c r="E32" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="O32" s="8"/>
     </row>
@@ -3123,26 +3124,26 @@
         <v>1</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
@@ -3151,7 +3152,7 @@
         <v>43</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="O33" s="8"/>
     </row>
@@ -3160,35 +3161,35 @@
         <v>7</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="O34" s="8"/>
     </row>
@@ -3197,38 +3198,38 @@
         <v>1</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
       <c r="M35" s="6" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="O35" s="8" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
@@ -3243,7 +3244,7 @@
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>29</v>
@@ -3273,14 +3274,14 @@
         <v>7</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>67</v>
@@ -3289,19 +3290,19 @@
         <v>68</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="O37" s="8"/>
     </row>
@@ -3310,51 +3311,51 @@
         <v>9</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F38" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G38" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G38" s="6" t="s">
-        <v>76</v>
-      </c>
       <c r="H38" s="6" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
       <c r="M38" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="O38" s="8"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>69</v>
+        <v>443</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>66</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>67</v>
@@ -3363,19 +3364,19 @@
         <v>68</v>
       </c>
       <c r="H39" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I39" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
       <c r="M39" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N39" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="N39" s="6" t="s">
-        <v>73</v>
       </c>
       <c r="O39" s="8"/>
     </row>
@@ -3384,35 +3385,35 @@
         <v>4</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>77</v>
+        <v>444</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F40" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G40" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="H40" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="H40" s="6" t="s">
-        <v>78</v>
-      </c>
       <c r="I40" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
       <c r="M40" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O40" s="8"/>
     </row>
@@ -3421,14 +3422,14 @@
         <v>18</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>94</v>
+        <v>445</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>67</v>
@@ -3437,19 +3438,19 @@
         <v>68</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
       <c r="M41" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="O41" s="8"/>
     </row>
@@ -3458,26 +3459,26 @@
         <v>6</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
@@ -3486,7 +3487,7 @@
         <v>35</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="O42" s="8"/>
     </row>
@@ -3495,14 +3496,14 @@
         <v>8</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>110</v>
+        <v>446</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>67</v>
@@ -3511,19 +3512,19 @@
         <v>68</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
       <c r="M43" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="O43" s="8"/>
     </row>
@@ -3532,35 +3533,35 @@
         <v>3</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>106</v>
+        <v>447</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F44" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="G44" s="6" t="s">
-        <v>76</v>
-      </c>
       <c r="H44" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
       <c r="M44" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="N44" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="O44" s="8"/>
     </row>
@@ -3569,14 +3570,14 @@
         <v>4</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>83</v>
+        <v>448</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>67</v>
@@ -3585,19 +3586,19 @@
         <v>68</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
       <c r="M45" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="O45" s="8"/>
     </row>
@@ -3606,14 +3607,14 @@
         <v>10</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>67</v>
@@ -3622,19 +3623,19 @@
         <v>68</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
       <c r="M46" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="O46" s="8"/>
     </row>
@@ -3643,14 +3644,14 @@
         <v>6</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>67</v>
@@ -3659,19 +3660,19 @@
         <v>68</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
       <c r="M47" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N47" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="O47" s="8"/>
     </row>
@@ -3680,16 +3681,16 @@
         <v>1</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>67</v>
@@ -3705,10 +3706,10 @@
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
       <c r="M48" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="O48" s="8"/>
     </row>
@@ -3717,72 +3718,72 @@
         <v>2</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
       <c r="M49" s="6" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="O49" s="8"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>313</v>
+        <v>458</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>311</v>
+        <v>272</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>311</v>
+        <v>272</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>312</v>
+        <v>272</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>315</v>
+        <v>274</v>
       </c>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
       <c r="M50" s="6" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>399</v>
+        <v>272</v>
       </c>
       <c r="O50" s="8"/>
     </row>
@@ -3791,183 +3792,183 @@
         <v>2</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>294</v>
+        <v>453</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
       <c r="M51" s="6" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="N51" s="6" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="O51" s="8"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
-        <v>1</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>318</v>
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>452</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
       <c r="M52" s="6" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>316</v>
+        <v>386</v>
       </c>
       <c r="O52" s="8"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>328</v>
+        <v>454</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="D53" s="7"/>
-      <c r="E53" s="7" t="s">
-        <v>382</v>
+      <c r="E53" s="5" t="s">
+        <v>368</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>327</v>
+        <v>308</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>329</v>
+        <v>309</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
       <c r="M53" s="6" t="s">
-        <v>287</v>
+        <v>387</v>
       </c>
       <c r="N53" s="6" t="s">
-        <v>403</v>
+        <v>307</v>
       </c>
       <c r="O53" s="8"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
-        <v>5</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>333</v>
+        <v>4</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>455</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>404</v>
+        <v>318</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
       <c r="M54" s="6" t="s">
-        <v>345</v>
+        <v>280</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="O54" s="8"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
-        <v>2</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>362</v>
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>456</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>361</v>
+        <v>320</v>
       </c>
       <c r="D55" s="7"/>
-      <c r="E55" s="5" t="s">
-        <v>381</v>
+      <c r="E55" s="7" t="s">
+        <v>369</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>361</v>
+        <v>320</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>361</v>
+        <v>321</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>363</v>
+        <v>391</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>364</v>
+        <v>322</v>
       </c>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
       <c r="M55" s="6" t="s">
-        <v>407</v>
+        <v>333</v>
       </c>
       <c r="N55" s="6" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="O55" s="8"/>
     </row>
@@ -3976,35 +3977,35 @@
         <v>2</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>279</v>
+        <v>457</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>278</v>
+        <v>349</v>
       </c>
       <c r="D56" s="7"/>
       <c r="E56" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>278</v>
+        <v>349</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>278</v>
+        <v>349</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>280</v>
+        <v>350</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>281</v>
+        <v>351</v>
       </c>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
       <c r="L56" s="6"/>
       <c r="M56" s="6" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>278</v>
+        <v>393</v>
       </c>
       <c r="O56" s="8"/>
     </row>
@@ -4013,38 +4014,38 @@
         <v>1</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
       <c r="L57" s="6"/>
       <c r="M57" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="N57" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="O57" s="8" t="s">
         <v>383</v>
-      </c>
-      <c r="N57" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="O57" s="8" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
@@ -4052,36 +4053,36 @@
         <v>4</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="7" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
       <c r="M58" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="O58" s="8" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
@@ -4089,32 +4090,32 @@
         <v>12</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
       <c r="L59" s="6"/>
       <c r="M59" s="6" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="N59" s="12">
         <v>5001</v>
@@ -4126,35 +4127,35 @@
         <v>6</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
       <c r="L60" s="6"/>
       <c r="M60" s="6" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="N60" s="6" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="O60" s="8"/>
     </row>
@@ -4163,35 +4164,35 @@
         <v>2</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
       <c r="L61" s="6"/>
       <c r="M61" s="6" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="N61" s="6" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="O61" s="8"/>
     </row>
@@ -4200,35 +4201,35 @@
         <v>1</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D62" s="7"/>
       <c r="E62" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
       <c r="L62" s="6"/>
       <c r="M62" s="6" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="N62" s="6" t="s">
-        <v>413</v>
+        <v>400</v>
       </c>
       <c r="O62" s="8"/>
     </row>
@@ -4237,35 +4238,35 @@
         <v>3</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="J63" s="6"/>
       <c r="K63" s="6"/>
       <c r="L63" s="6"/>
       <c r="M63" s="6" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="N63" s="6" t="s">
-        <v>416</v>
+        <v>403</v>
       </c>
       <c r="O63" s="8"/>
     </row>
@@ -4274,35 +4275,35 @@
         <v>1</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
       <c r="M64" s="6" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="N64" s="6" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="O64" s="8"/>
     </row>
@@ -4311,35 +4312,35 @@
         <v>1</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="J65" s="6"/>
       <c r="K65" s="6"/>
       <c r="L65" s="6"/>
       <c r="M65" s="6" t="s">
-        <v>419</v>
+        <v>406</v>
       </c>
       <c r="N65" s="6" t="s">
-        <v>418</v>
+        <v>405</v>
       </c>
       <c r="O65" s="8"/>
     </row>
@@ -4348,35 +4349,35 @@
         <v>1</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
       <c r="J66" s="6"/>
       <c r="K66" s="6"/>
       <c r="L66" s="6"/>
       <c r="M66" s="6" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="O66" s="8"/>
     </row>
@@ -4385,35 +4386,35 @@
         <v>1</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="J67" s="6"/>
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
       <c r="M67" s="6" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="N67" s="6" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="O67" s="8"/>
     </row>
@@ -4422,35 +4423,35 @@
         <v>3</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="J68" s="6"/>
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
       <c r="M68" s="6" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="N68" s="6" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="O68" s="8"/>
     </row>
@@ -4459,38 +4460,38 @@
         <v>2</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="5" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
       <c r="M69" s="6" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="N69" s="6" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="O69" s="4" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
@@ -4498,35 +4499,35 @@
         <v>1</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D70" s="7"/>
       <c r="E70" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="J70" s="6"/>
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
       <c r="M70" s="6" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="N70" s="6" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="O70" s="8"/>
     </row>
@@ -4535,35 +4536,35 @@
         <v>1</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="J71" s="6"/>
       <c r="K71" s="6"/>
       <c r="L71" s="6"/>
       <c r="M71" s="6" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="N71" s="6" t="s">
-        <v>427</v>
+        <v>414</v>
       </c>
       <c r="O71" s="8"/>
     </row>
@@ -4572,35 +4573,35 @@
         <v>4</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
       <c r="L72" s="6"/>
       <c r="M72" s="6" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="N72" s="6" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
       <c r="O72" s="8"/>
     </row>
@@ -4609,35 +4610,35 @@
         <v>3</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="I73" s="6" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="J73" s="6"/>
       <c r="K73" s="6"/>
       <c r="L73" s="6"/>
       <c r="M73" s="6" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="N73" s="6" t="s">
-        <v>429</v>
+        <v>416</v>
       </c>
       <c r="O73" s="8"/>
     </row>
@@ -4646,35 +4647,35 @@
         <v>2</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="I74" s="6" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="J74" s="6"/>
       <c r="K74" s="6"/>
       <c r="L74" s="6"/>
       <c r="M74" s="6" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="N74" s="6" t="s">
-        <v>430</v>
+        <v>417</v>
       </c>
       <c r="O74" s="8"/>
     </row>
@@ -4683,35 +4684,35 @@
         <v>2</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I75" s="6" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J75" s="6"/>
       <c r="K75" s="6"/>
       <c r="L75" s="6"/>
       <c r="M75" s="6" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="N75" s="6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="O75" s="8"/>
     </row>
@@ -4720,46 +4721,46 @@
         <v>1</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="7" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="J76" s="6"/>
       <c r="K76" s="6"/>
       <c r="L76" s="6"/>
       <c r="M76" s="6" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="N76" s="6" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="O76" s="8"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B79" s="13" t="s">
-        <v>377</v>
-      </c>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="13"/>
+      <c r="B79" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
     </row>
   </sheetData>
   <sortState ref="A2:S76">

</xml_diff>